<commit_message>
Fixed data, added availability
</commit_message>
<xml_diff>
--- a/src/WebMarket/WebMarket/App_Data/CurrentRelay.xlsx
+++ b/src/WebMarket/WebMarket/App_Data/CurrentRelay.xlsx
@@ -8,13 +8,14 @@
   </bookViews>
   <sheets>
     <sheet name="CurrentRelay" sheetId="1" r:id="rId1"/>
+    <sheet name="Metadata" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="39">
   <si>
     <t>50A</t>
   </si>
@@ -122,6 +123,15 @@
   </si>
   <si>
     <t>Максимальный ток перегрузки=80 А&amp;Выход реле=1 переключающий контакт&amp;Максимальный ток на контактах реле=не более 6 A&amp;Степень защиты прибора=IP20&amp;Сечение силовых клемм=16 мм2</t>
+  </si>
+  <si>
+    <t>24.07.2013</t>
+  </si>
+  <si>
+    <t>01.08.2012</t>
+  </si>
+  <si>
+    <t>Price update</t>
   </si>
 </sst>
 </file>
@@ -462,8 +472,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="Q4" sqref="Q4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P26" sqref="P26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -551,7 +561,7 @@
         <v>4</v>
       </c>
       <c r="B2">
-        <v>256</v>
+        <v>244</v>
       </c>
       <c r="D2" t="b">
         <v>1</v>
@@ -597,6 +607,40 @@
       </c>
       <c r="X2" t="s">
         <v>34</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.28515625" customWidth="1"/>
+    <col min="2" max="2" width="12.140625" customWidth="1"/>
+    <col min="3" max="3" width="18.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>